<commit_message>
another step in the excel, improved styling, dataparse, color is added to the name
</commit_message>
<xml_diff>
--- a/clean.xlsx
+++ b/clean.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Ramon\Desktop\cursojs\AdminR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\Ramon\Desktop\cursojs\AdminR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -373,7 +373,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +694,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -927,7 +935,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1185,14 +1193,22 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="41" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="43" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="43" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2211,14 +2227,14 @@
   </sheetPr>
   <dimension ref="B4:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="47" style="7" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" style="11" customWidth="1"/>
@@ -2243,7 +2259,7 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E7" s="203"/>
+      <c r="E7" s="208"/>
     </row>
     <row r="8" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="22" t="s">
@@ -2292,12 +2308,12 @@
       <c r="B12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="204"/>
-      <c r="D12" s="204" t="s">
+      <c r="C12" s="203"/>
+      <c r="D12" s="203" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="208"/>
-      <c r="F12" s="206"/>
+      <c r="E12" s="206"/>
+      <c r="F12" s="205"/>
       <c r="I12"/>
       <c r="J12" s="67"/>
     </row>
@@ -2305,22 +2321,22 @@
       <c r="B13" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="204"/>
-      <c r="D13" s="204" t="s">
+      <c r="C13" s="203"/>
+      <c r="D13" s="203" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="207"/>
-      <c r="F13" s="206"/>
+      <c r="F13" s="205"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="204" t="s">
+      <c r="B14" s="203" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="205"/>
-      <c r="D14" s="205"/>
-      <c r="E14" s="206"/>
-      <c r="F14" s="206"/>
+      <c r="C14" s="204"/>
+      <c r="D14" s="204"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="205"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
@@ -2364,7 +2380,10 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="202"/>
       <c r="C20" s="202"/>
+      <c r="D20" s="202"/>
+      <c r="E20" s="209"/>
       <c r="F20" s="8" t="str">
         <f t="shared" ref="F20:F33" si="0">IF(D20&lt;&gt;"",D20*E20,"")</f>
         <v/>
@@ -2391,7 +2410,10 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="202"/>
       <c r="C23" s="202"/>
+      <c r="D23" s="202"/>
+      <c r="E23" s="209"/>
       <c r="F23" s="8" t="str">
         <f>IF(D23&lt;&gt;"",D23*E23,"")</f>
         <v/>
@@ -2418,7 +2440,10 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="202"/>
       <c r="C26" s="202"/>
+      <c r="D26" s="202"/>
+      <c r="E26" s="209"/>
       <c r="F26" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2427,7 +2452,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
-      <c r="C27"/>
+      <c r="C27" s="210"/>
       <c r="D27" s="31"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="str">
@@ -2446,7 +2471,10 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="202"/>
       <c r="C29" s="202"/>
+      <c r="D29" s="202"/>
+      <c r="E29" s="209"/>
       <c r="F29" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2473,7 +2501,10 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="202"/>
       <c r="C32" s="202"/>
+      <c r="D32" s="202"/>
+      <c r="E32" s="209"/>
       <c r="F32" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2481,7 +2512,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
-      <c r="C33"/>
+      <c r="C33" s="210"/>
       <c r="D33" s="31"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="str">
@@ -2540,10 +2571,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="35">
-        <v>17</v>
+        <v>0.33</v>
       </c>
       <c r="F37" s="35">
-        <f>D37*E37</f>
+        <f>IF(D37*E37&lt;17, 17,D37*E37)</f>
         <v>17</v>
       </c>
     </row>

</xml_diff>